<commit_message>
Reloaded meter_readings table from new Excel, improved reload script, and deleted one-off script after use
</commit_message>
<xml_diff>
--- a/meter_ref_data.xlsx
+++ b/meter_ref_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishekpan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A88BFA-5395-A344-B008-55BDF05A26AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF93442E-B271-5F4B-B17E-4077B28B595A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{D1BA573D-F61D-E94C-8400-4F4191A4CCC6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>meter_serial_number</t>
   </si>
@@ -46,9 +46,6 @@
     <t>reading_date</t>
   </si>
   <si>
-    <t>reading unit</t>
-  </si>
-  <si>
     <t>kWh</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>004420</t>
   </si>
   <si>
-    <t>21043</t>
-  </si>
-  <si>
     <t>N-002465</t>
   </si>
   <si>
@@ -115,13 +109,28 @@
     <t>016067</t>
   </si>
   <si>
-    <t>90965</t>
-  </si>
-  <si>
     <t>01810142</t>
   </si>
   <si>
     <t>018289</t>
+  </si>
+  <si>
+    <t>090965</t>
+  </si>
+  <si>
+    <t>01809383</t>
+  </si>
+  <si>
+    <t>039672</t>
+  </si>
+  <si>
+    <t>021043</t>
+  </si>
+  <si>
+    <t>kWH</t>
+  </si>
+  <si>
+    <t>reading_unit</t>
   </si>
 </sst>
 </file>
@@ -478,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA76C4E-E2F0-734E-BAF1-92DB787B8996}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -507,41 +516,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
-        <v>44848.427488425928</v>
+        <v>44848.428611111114</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
-        <v>44838.428194444445</v>
+        <v>44848.427488425928</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1">
         <v>44838.430069444446</v>
@@ -549,13 +558,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
         <v>44838.429224537038</v>
@@ -563,13 +572,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>44838.433668981481</v>
@@ -577,13 +586,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>44838.43440972222</v>
@@ -591,13 +600,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1">
         <v>44838.433298611111</v>
@@ -605,13 +614,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
         <v>44838.433506944442</v>
@@ -619,13 +628,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1">
         <v>44838.433993055558</v>
@@ -633,13 +642,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
         <v>44838.434247685182</v>
@@ -647,13 +656,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1">
         <v>44838.434618055559</v>
@@ -661,16 +670,30 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1">
         <v>44838.924074074072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44838.428194444445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>